<commit_message>
modified the code to look perfect. It works great. Working as expected
</commit_message>
<xml_diff>
--- a/mystockholdings.xlsx
+++ b/mystockholdings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Stock</t>
   </si>
@@ -31,12 +31,6 @@
     <t>Current Price</t>
   </si>
   <si>
-    <t>Gain or Loss</t>
-  </si>
-  <si>
-    <t>Percentage</t>
-  </si>
-  <si>
     <t>Todays Change</t>
   </si>
   <si>
@@ -59,6 +53,18 @@
   </si>
   <si>
     <t>NTNX</t>
+  </si>
+  <si>
+    <t>AVXL</t>
+  </si>
+  <si>
+    <t>VTV</t>
+  </si>
+  <si>
+    <t>XLK</t>
+  </si>
+  <si>
+    <t>TSM</t>
   </si>
 </sst>
 </file>
@@ -416,13 +422,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,107 +459,217 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
       <c r="B2">
-        <v>90</v>
+        <v>31.73</v>
       </c>
       <c r="C2">
-        <v>800</v>
+        <v>844.58</v>
       </c>
       <c r="D2">
-        <v>72000</v>
+        <v>26798.5234</v>
       </c>
       <c r="E2">
         <v>8.619999885559082</v>
       </c>
+      <c r="F2">
+        <v>-0.130000114440918</v>
+      </c>
+      <c r="G2">
+        <v>-1.49</v>
+      </c>
       <c r="H2">
-        <v>-0.130000114440918</v>
+        <v>-19518.24389665451</v>
       </c>
       <c r="I2">
-        <v>-1.49</v>
+        <v>-72.83328116747848</v>
       </c>
       <c r="J2">
-        <v>-65104.00009155273</v>
-      </c>
-      <c r="K2">
-        <v>-90.4222223493788</v>
-      </c>
-      <c r="L2">
         <v>-7.809262812769592</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3">
-        <v>90</v>
+        <v>90.94</v>
       </c>
       <c r="C3">
-        <v>600</v>
+        <v>360</v>
       </c>
       <c r="D3">
-        <v>54000</v>
+        <v>32738.4</v>
       </c>
       <c r="E3">
         <v>35.06999969482422</v>
       </c>
+      <c r="F3">
+        <v>0.6399993896484375</v>
+      </c>
+      <c r="G3">
+        <v>1.86</v>
+      </c>
       <c r="H3">
-        <v>0.6399993896484375</v>
+        <v>-20113.20010986328</v>
       </c>
       <c r="I3">
-        <v>1.86</v>
+        <v>-61.43611205759377</v>
       </c>
       <c r="J3">
-        <v>-32958.00018310547</v>
-      </c>
-      <c r="K3">
-        <v>-61.03333367241753</v>
-      </c>
-      <c r="L3">
         <v>-7.809262812769592</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4">
-        <v>73</v>
+        <v>73.16</v>
       </c>
       <c r="C4">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="D4">
-        <v>14600</v>
+        <v>12803</v>
       </c>
       <c r="E4">
         <v>66.69999694824219</v>
       </c>
+      <c r="F4">
+        <v>-5.650001525878906</v>
+      </c>
+      <c r="G4">
+        <v>-7.81</v>
+      </c>
       <c r="H4">
-        <v>-5.650001525878906</v>
+        <v>-1130.500534057617</v>
       </c>
       <c r="I4">
-        <v>-7.81</v>
+        <v>-8.829965899067536</v>
       </c>
       <c r="J4">
-        <v>-1260.000610351562</v>
-      </c>
-      <c r="K4">
-        <v>-8.630141166791525</v>
-      </c>
-      <c r="L4">
         <v>-7.809262812769592</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>6.21</v>
+      </c>
+      <c r="C5">
+        <v>2065</v>
+      </c>
+      <c r="D5">
+        <v>12823.65</v>
+      </c>
+      <c r="E5">
+        <v>9.029999732971191</v>
+      </c>
+      <c r="F5">
+        <v>-0.005000114440917969</v>
+      </c>
+      <c r="G5">
+        <v>-0.06</v>
+      </c>
+      <c r="H5">
+        <v>5823.299448585511</v>
+      </c>
+      <c r="I5">
+        <v>45.41062371934286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>179.95</v>
+      </c>
+      <c r="C6">
+        <v>75</v>
+      </c>
+      <c r="D6">
+        <v>13496.25</v>
+      </c>
+      <c r="E6">
+        <v>181.2599945068359</v>
+      </c>
+      <c r="F6">
+        <v>-0.0800018310546875</v>
+      </c>
+      <c r="G6">
+        <v>-0.04</v>
+      </c>
+      <c r="H6">
+        <v>98.24958801269617</v>
+      </c>
+      <c r="I6">
+        <v>0.7279769418371486</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>234.42</v>
+      </c>
+      <c r="C7">
+        <v>135</v>
+      </c>
+      <c r="D7">
+        <v>31646.7</v>
+      </c>
+      <c r="E7">
+        <v>231.5800018310547</v>
+      </c>
+      <c r="F7">
+        <v>-3.17999267578125</v>
+      </c>
+      <c r="G7">
+        <v>-1.35</v>
+      </c>
+      <c r="H7">
+        <v>-383.3997528076155</v>
+      </c>
+      <c r="I7">
+        <v>-1.211499944094062</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>193.64</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>2323.68</v>
+      </c>
+      <c r="E8">
+        <v>181.1900024414062</v>
+      </c>
+      <c r="F8">
+        <v>-2.649993896484375</v>
+      </c>
+      <c r="G8">
+        <v>-1.44</v>
+      </c>
+      <c r="H8">
+        <v>-149.3999707031248</v>
+      </c>
+      <c r="I8">
+        <v>-6.429455463020934</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added gitignore for the excel file
</commit_message>
<xml_diff>
--- a/mystockholdings.xlsx
+++ b/mystockholdings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Stock</t>
   </si>
@@ -31,21 +31,18 @@
     <t>Current Price</t>
   </si>
   <si>
+    <t>Profit/Loss</t>
+  </si>
+  <si>
+    <t>Percentage Change</t>
+  </si>
+  <si>
     <t>Todays Change</t>
   </si>
   <si>
     <t>Todays Change Percent</t>
   </si>
   <si>
-    <t>Profit/Loss</t>
-  </si>
-  <si>
-    <t>Percentage Change</t>
-  </si>
-  <si>
-    <t>Change Percent</t>
-  </si>
-  <si>
     <t>NVAX</t>
   </si>
   <si>
@@ -56,9 +53,6 @@
   </si>
   <si>
     <t>AVXL</t>
-  </si>
-  <si>
-    <t>VTV</t>
   </si>
   <si>
     <t>XLK</t>
@@ -422,13 +416,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,13 +450,10 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>10</v>
       </c>
       <c r="B2">
         <v>31.73</v>
@@ -474,27 +465,24 @@
         <v>26798.5234</v>
       </c>
       <c r="E2">
-        <v>8.619999885559082</v>
+        <v>8.659999847412109</v>
       </c>
       <c r="F2">
-        <v>-0.130000114440918</v>
+        <v>-19484.46072887268</v>
       </c>
       <c r="G2">
-        <v>-1.49</v>
+        <v>-72.70721762555276</v>
       </c>
       <c r="H2">
-        <v>-19518.24389665451</v>
+        <v>-0.1100006103515625</v>
       </c>
       <c r="I2">
-        <v>-72.83328116747848</v>
-      </c>
-      <c r="J2">
-        <v>-7.809262812769592</v>
+        <v>-1.25</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>90.94</v>
@@ -506,27 +494,24 @@
         <v>32738.4</v>
       </c>
       <c r="E3">
-        <v>35.06999969482422</v>
+        <v>41.59999847412109</v>
       </c>
       <c r="F3">
-        <v>0.6399993896484375</v>
+        <v>-17762.4005493164</v>
       </c>
       <c r="G3">
-        <v>1.86</v>
+        <v>-54.25555478983826</v>
       </c>
       <c r="H3">
-        <v>-20113.20010986328</v>
+        <v>-0.4000015258789062</v>
       </c>
       <c r="I3">
-        <v>-61.43611205759377</v>
-      </c>
-      <c r="J3">
-        <v>-7.809262812769592</v>
+        <v>-0.95</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>73.16</v>
@@ -538,27 +523,24 @@
         <v>12803</v>
       </c>
       <c r="E4">
-        <v>66.69999694824219</v>
+        <v>65.34999847412109</v>
       </c>
       <c r="F4">
-        <v>-5.650001525878906</v>
+        <v>-1366.750267028808</v>
       </c>
       <c r="G4">
-        <v>-7.81</v>
+        <v>-10.67523445308762</v>
       </c>
       <c r="H4">
-        <v>-1130.500534057617</v>
+        <v>-0.8000030517578125</v>
       </c>
       <c r="I4">
-        <v>-8.829965899067536</v>
-      </c>
-      <c r="J4">
-        <v>-7.809262812769592</v>
+        <v>-1.21</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>6.21</v>
@@ -570,106 +552,77 @@
         <v>12823.65</v>
       </c>
       <c r="E5">
-        <v>9.029999732971191</v>
+        <v>8.970000267028809</v>
       </c>
       <c r="F5">
-        <v>-0.005000114440917969</v>
+        <v>5699.40055141449</v>
       </c>
       <c r="G5">
-        <v>-0.06</v>
+        <v>44.44444874442526</v>
       </c>
       <c r="H5">
-        <v>5823.299448585511</v>
+        <v>-0.3499994277954102</v>
       </c>
       <c r="I5">
-        <v>45.41062371934286</v>
+        <v>-3.76</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>234.6</v>
+      </c>
+      <c r="C6">
+        <v>156.21</v>
+      </c>
+      <c r="D6">
+        <v>36646.866</v>
+      </c>
+      <c r="E6">
+        <v>235.9001007080078</v>
+      </c>
+      <c r="F6">
+        <v>203.0887315979013</v>
+      </c>
+      <c r="G6">
+        <v>0.5541776248967683</v>
+      </c>
+      <c r="H6">
+        <v>-0.049896240234375</v>
+      </c>
+      <c r="I6">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B6">
-        <v>179.95</v>
-      </c>
-      <c r="C6">
-        <v>75</v>
-      </c>
-      <c r="D6">
-        <v>13496.25</v>
-      </c>
-      <c r="E6">
-        <v>181.2599945068359</v>
-      </c>
-      <c r="F6">
-        <v>-0.0800018310546875</v>
-      </c>
-      <c r="G6">
-        <v>-0.04</v>
-      </c>
-      <c r="H6">
-        <v>98.24958801269617</v>
-      </c>
-      <c r="I6">
-        <v>0.7279769418371486</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
       <c r="B7">
-        <v>234.42</v>
+        <v>188.22</v>
       </c>
       <c r="C7">
-        <v>135</v>
+        <v>24.09</v>
       </c>
       <c r="D7">
-        <v>31646.7</v>
+        <v>4534.2198</v>
       </c>
       <c r="E7">
-        <v>231.5800018310547</v>
+        <v>197.7149963378906</v>
       </c>
       <c r="F7">
-        <v>-3.17999267578125</v>
+        <v>228.7344617797852</v>
       </c>
       <c r="G7">
-        <v>-1.35</v>
+        <v>5.04462668042218</v>
       </c>
       <c r="H7">
-        <v>-383.3997528076155</v>
+        <v>3.31500244140625</v>
       </c>
       <c r="I7">
-        <v>-1.211499944094062</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8">
-        <v>193.64</v>
-      </c>
-      <c r="C8">
-        <v>12</v>
-      </c>
-      <c r="D8">
-        <v>2323.68</v>
-      </c>
-      <c r="E8">
-        <v>181.1900024414062</v>
-      </c>
-      <c r="F8">
-        <v>-2.649993896484375</v>
-      </c>
-      <c r="G8">
-        <v>-1.44</v>
-      </c>
-      <c r="H8">
-        <v>-149.3999707031248</v>
-      </c>
-      <c r="I8">
-        <v>-6.429455463020934</v>
+        <v>1.71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified to Separate Stock and ETF
</commit_message>
<xml_diff>
--- a/mystockholdings.xlsx
+++ b/mystockholdings.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+  <si>
+    <t>Type</t>
+  </si>
   <si>
     <t>Stock</t>
   </si>
@@ -43,6 +46,12 @@
     <t>Todays Change Percent</t>
   </si>
   <si>
+    <t>stock</t>
+  </si>
+  <si>
+    <t>etf</t>
+  </si>
+  <si>
     <t>NVAX</t>
   </si>
   <si>
@@ -55,10 +64,28 @@
     <t>AVXL</t>
   </si>
   <si>
-    <t>XLK</t>
-  </si>
-  <si>
-    <t>TSM</t>
+    <t>NVDA</t>
+  </si>
+  <si>
+    <t>SMH</t>
+  </si>
+  <si>
+    <t>VOOG</t>
+  </si>
+  <si>
+    <t>VTV</t>
+  </si>
+  <si>
+    <t>XLU</t>
+  </si>
+  <si>
+    <t>VFH</t>
+  </si>
+  <si>
+    <t>SCHG</t>
+  </si>
+  <si>
+    <t>IGPT</t>
   </si>
 </sst>
 </file>
@@ -416,13 +443,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,179 +477,392 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
         <v>31.73</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>844.58</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>26798.5234</v>
       </c>
-      <c r="E2">
-        <v>8.659999847412109</v>
-      </c>
       <c r="F2">
-        <v>-19484.46072887268</v>
+        <v>8.359999656677246</v>
       </c>
       <c r="G2">
-        <v>-72.70721762555276</v>
+        <v>-19737.83488996353</v>
       </c>
       <c r="H2">
-        <v>-0.1100006103515625</v>
+        <v>-73.65269569279154</v>
       </c>
       <c r="I2">
-        <v>-1.25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>-0.07000064849853516</v>
+      </c>
+      <c r="J2">
+        <v>-0.83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>90.94</v>
+      <c r="B3" t="s">
+        <v>13</v>
       </c>
       <c r="C3">
-        <v>360</v>
+        <v>72.11</v>
       </c>
       <c r="D3">
-        <v>32738.4</v>
+        <v>595</v>
       </c>
       <c r="E3">
-        <v>41.59999847412109</v>
+        <v>42905.45</v>
       </c>
       <c r="F3">
-        <v>-17762.4005493164</v>
+        <v>28.81999969482422</v>
       </c>
       <c r="G3">
-        <v>-54.25555478983826</v>
+        <v>-25757.55018157959</v>
       </c>
       <c r="H3">
-        <v>-0.4000015258789062</v>
+        <v>-60.0332829083009</v>
       </c>
       <c r="I3">
-        <v>-0.95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>1.969999313354492</v>
+      </c>
+      <c r="J3">
+        <v>7.34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>73.16</v>
+      </c>
+      <c r="D4">
+        <v>175</v>
+      </c>
+      <c r="E4">
+        <v>12803</v>
+      </c>
+      <c r="F4">
+        <v>70.44499969482422</v>
+      </c>
+      <c r="G4">
+        <v>-475.1250534057612</v>
+      </c>
+      <c r="H4">
+        <v>-3.711044703630095</v>
+      </c>
+      <c r="I4">
+        <v>1.675003051757812</v>
+      </c>
+      <c r="J4">
+        <v>2.44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>6.21</v>
+      </c>
+      <c r="D5">
+        <v>2065</v>
+      </c>
+      <c r="E5">
+        <v>12823.65</v>
+      </c>
+      <c r="F5">
+        <v>8.939999580383301</v>
+      </c>
+      <c r="G5">
+        <v>5637.449133491516</v>
+      </c>
+      <c r="H5">
+        <v>43.96134589989212</v>
+      </c>
+      <c r="I5">
+        <v>0.2999992370605469</v>
+      </c>
+      <c r="J5">
+        <v>3.47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>144.47</v>
+      </c>
+      <c r="D6">
+        <v>293</v>
+      </c>
+      <c r="E6">
+        <v>42329.71</v>
+      </c>
+      <c r="F6">
+        <v>118.629997253418</v>
+      </c>
+      <c r="G6">
+        <v>-7571.120804748535</v>
+      </c>
+      <c r="H6">
+        <v>-17.88606821248842</v>
+      </c>
+      <c r="I6">
+        <v>1.969993591308594</v>
+      </c>
+      <c r="J6">
+        <v>1.69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
-        <v>73.16</v>
-      </c>
-      <c r="C4">
-        <v>175</v>
-      </c>
-      <c r="D4">
-        <v>12803</v>
-      </c>
-      <c r="E4">
-        <v>65.34999847412109</v>
-      </c>
-      <c r="F4">
-        <v>-1366.750267028808</v>
-      </c>
-      <c r="G4">
-        <v>-10.67523445308762</v>
-      </c>
-      <c r="H4">
-        <v>-0.8000030517578125</v>
-      </c>
-      <c r="I4">
-        <v>-1.21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>6.21</v>
-      </c>
-      <c r="C5">
-        <v>2065</v>
-      </c>
-      <c r="D5">
-        <v>12823.65</v>
-      </c>
-      <c r="E5">
-        <v>8.970000267028809</v>
-      </c>
-      <c r="F5">
-        <v>5699.40055141449</v>
-      </c>
-      <c r="G5">
-        <v>44.44444874442526</v>
-      </c>
-      <c r="H5">
-        <v>-0.3499994277954102</v>
-      </c>
-      <c r="I5">
-        <v>-3.76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6">
-        <v>234.6</v>
-      </c>
-      <c r="C6">
-        <v>156.21</v>
-      </c>
-      <c r="D6">
-        <v>36646.866</v>
-      </c>
-      <c r="E6">
-        <v>235.9001007080078</v>
-      </c>
-      <c r="F6">
-        <v>203.0887315979013</v>
-      </c>
-      <c r="G6">
-        <v>0.5541776248967683</v>
-      </c>
-      <c r="H6">
-        <v>-0.049896240234375</v>
-      </c>
-      <c r="I6">
-        <v>-0.02</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7">
-        <v>188.22</v>
+      <c r="B7" t="s">
+        <v>17</v>
       </c>
       <c r="C7">
-        <v>24.09</v>
+        <v>244.94</v>
       </c>
       <c r="D7">
-        <v>4534.2198</v>
+        <v>118.664</v>
       </c>
       <c r="E7">
-        <v>197.7149963378906</v>
+        <v>29065.56016</v>
       </c>
       <c r="F7">
-        <v>228.7344617797852</v>
+        <v>240.8999938964844</v>
       </c>
       <c r="G7">
-        <v>5.04462668042218</v>
+        <v>-479.4032842675779</v>
       </c>
       <c r="H7">
-        <v>3.31500244140625</v>
+        <v>-1.649386014336418</v>
       </c>
       <c r="I7">
-        <v>1.71</v>
+        <v>2.1199951171875</v>
+      </c>
+      <c r="J7">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>323.66</v>
+      </c>
+      <c r="D8">
+        <v>22.81</v>
+      </c>
+      <c r="E8">
+        <v>7382.684600000001</v>
+      </c>
+      <c r="F8">
+        <v>375.25</v>
+      </c>
+      <c r="G8">
+        <v>1176.767899999999</v>
+      </c>
+      <c r="H8">
+        <v>15.93956621145646</v>
+      </c>
+      <c r="I8">
+        <v>2.6400146484375</v>
+      </c>
+      <c r="J8">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>178.95</v>
+      </c>
+      <c r="D9">
+        <v>25</v>
+      </c>
+      <c r="E9">
+        <v>4473.75</v>
+      </c>
+      <c r="F9">
+        <v>176.0950012207031</v>
+      </c>
+      <c r="G9">
+        <v>-71.37496948242159</v>
+      </c>
+      <c r="H9">
+        <v>-1.595417032297773</v>
+      </c>
+      <c r="I9">
+        <v>-0.084991455078125</v>
+      </c>
+      <c r="J9">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>78.95999999999999</v>
+      </c>
+      <c r="D10">
+        <v>1.267</v>
+      </c>
+      <c r="E10">
+        <v>100.04232</v>
+      </c>
+      <c r="F10">
+        <v>77.73500061035156</v>
+      </c>
+      <c r="G10">
+        <v>-1.552074226684562</v>
+      </c>
+      <c r="H10">
+        <v>-1.551417666728003</v>
+      </c>
+      <c r="I10">
+        <v>-0.56500244140625</v>
+      </c>
+      <c r="J10">
+        <v>-0.72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>124.23</v>
+      </c>
+      <c r="D11">
+        <v>0.805</v>
+      </c>
+      <c r="E11">
+        <v>100.00515</v>
+      </c>
+      <c r="F11">
+        <v>125.0786972045898</v>
+      </c>
+      <c r="G11">
+        <v>0.6832012496948211</v>
+      </c>
+      <c r="H11">
+        <v>0.6831660666423889</v>
+      </c>
+      <c r="I11">
+        <v>-0.051300048828125</v>
+      </c>
+      <c r="J11">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12">
+        <v>28.93</v>
+      </c>
+      <c r="D12">
+        <v>3.457</v>
+      </c>
+      <c r="E12">
+        <v>100.01101</v>
+      </c>
+      <c r="F12">
+        <v>28.41500091552734</v>
+      </c>
+      <c r="G12">
+        <v>-1.780351835021972</v>
+      </c>
+      <c r="H12">
+        <v>-1.780155839864002</v>
+      </c>
+      <c r="I12">
+        <v>0.2550010681152344</v>
+      </c>
+      <c r="J12">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13">
+        <v>48.94</v>
+      </c>
+      <c r="D13">
+        <v>2.042</v>
+      </c>
+      <c r="E13">
+        <v>99.93547999999998</v>
+      </c>
+      <c r="F13">
+        <v>47.20009994506836</v>
+      </c>
+      <c r="G13">
+        <v>-3.552875912170405</v>
+      </c>
+      <c r="H13">
+        <v>-3.555169707665792</v>
+      </c>
+      <c r="I13">
+        <v>0.3700981140136719</v>
+      </c>
+      <c r="J13">
+        <v>0.79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made some UI changes
</commit_message>
<xml_diff>
--- a/mystockholdings.xlsx
+++ b/mystockholdings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Type</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>IGPT</t>
+  </si>
+  <si>
+    <t>AMZN</t>
+  </si>
+  <si>
+    <t>VOO</t>
   </si>
 </sst>
 </file>
@@ -443,7 +449,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -498,19 +504,19 @@
         <v>26798.5234</v>
       </c>
       <c r="F2">
-        <v>8.645000457763672</v>
+        <v>7.929999828338623</v>
       </c>
       <c r="G2">
-        <v>-19497.12891338196</v>
+        <v>-20101.00414498177</v>
       </c>
       <c r="H2">
-        <v>-72.75448957527995</v>
+        <v>-75.00787951989089</v>
       </c>
       <c r="I2">
-        <v>0.2050008773803711</v>
+        <v>0.09999990463256836</v>
       </c>
       <c r="J2">
-        <v>2.43</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -530,19 +536,19 @@
         <v>42905.45</v>
       </c>
       <c r="F3">
-        <v>31.6298999786377</v>
+        <v>41.34999847412109</v>
       </c>
       <c r="G3">
-        <v>-24085.65951271057</v>
+        <v>-18302.20090789795</v>
       </c>
       <c r="H3">
-        <v>-56.13659689552393</v>
+        <v>-42.65705384257233</v>
       </c>
       <c r="I3">
-        <v>2.469900131225586</v>
+        <v>1.669998168945312</v>
       </c>
       <c r="J3">
-        <v>8.470000000000001</v>
+        <v>4.21</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -562,19 +568,19 @@
         <v>12803</v>
       </c>
       <c r="F4">
-        <v>71.51190185546875</v>
+        <v>70.73090362548828</v>
       </c>
       <c r="G4">
-        <v>-288.4171752929682</v>
+        <v>-425.0918655395502</v>
       </c>
       <c r="H4">
-        <v>-2.252731198101759</v>
+        <v>-3.320252015461612</v>
       </c>
       <c r="I4">
-        <v>0.5718994140625</v>
+        <v>0.4509048461914062</v>
       </c>
       <c r="J4">
-        <v>0.8100000000000001</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -594,19 +600,19 @@
         <v>12823.65</v>
       </c>
       <c r="F5">
-        <v>8.890000343322754</v>
+        <v>8.569999694824219</v>
       </c>
       <c r="G5">
-        <v>5534.200708961487</v>
+        <v>4873.399369812012</v>
       </c>
       <c r="H5">
-        <v>43.15620520648557</v>
+        <v>38.00321569765248</v>
       </c>
       <c r="I5">
-        <v>0.02000045776367188</v>
+        <v>-0.130000114440918</v>
       </c>
       <c r="J5">
-        <v>0.23</v>
+        <v>-1.49</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -626,19 +632,19 @@
         <v>42329.71</v>
       </c>
       <c r="F6">
-        <v>123.8000030517578</v>
+        <v>135.4100036621094</v>
       </c>
       <c r="G6">
-        <v>-6056.309105834961</v>
+        <v>-2654.578927001953</v>
       </c>
       <c r="H6">
-        <v>-14.30746656623672</v>
+        <v>-6.271195637772981</v>
       </c>
       <c r="I6">
-        <v>5.150001525878906</v>
+        <v>4.270004272460938</v>
       </c>
       <c r="J6">
-        <v>4.34</v>
+        <v>3.26</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -658,19 +664,19 @@
         <v>29065.56016</v>
       </c>
       <c r="F7">
-        <v>246.4600067138672</v>
+        <v>251.1300048828125</v>
       </c>
       <c r="G7">
-        <v>180.3700766943362</v>
+        <v>734.5307394140627</v>
       </c>
       <c r="H7">
-        <v>0.6205628782016779</v>
+        <v>2.527151499474362</v>
       </c>
       <c r="I7">
-        <v>4.990005493164062</v>
+        <v>2.620010375976562</v>
       </c>
       <c r="J7">
-        <v>2.07</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -690,19 +696,19 @@
         <v>7382.684600000001</v>
       </c>
       <c r="F8">
-        <v>377.4549865722656</v>
+        <v>382.2099914550781</v>
       </c>
       <c r="G8">
-        <v>1227.063643713378</v>
+        <v>1335.525305090331</v>
       </c>
       <c r="H8">
-        <v>16.62083253175109</v>
+        <v>18.08996831708524</v>
       </c>
       <c r="I8">
-        <v>0.7349853515625</v>
+        <v>3.25</v>
       </c>
       <c r="J8">
-        <v>0.2</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -722,19 +728,19 @@
         <v>4473.75</v>
       </c>
       <c r="F9">
-        <v>177.5350036621094</v>
+        <v>177.0099945068359</v>
       </c>
       <c r="G9">
-        <v>-35.37490844726534</v>
+        <v>-48.50013732910128</v>
       </c>
       <c r="H9">
-        <v>-0.790721619385646</v>
+        <v>-1.084104774050881</v>
       </c>
       <c r="I9">
-        <v>1.355010986328125</v>
+        <v>0.5099945068359375</v>
       </c>
       <c r="J9">
-        <v>0.77</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -754,19 +760,19 @@
         <v>100.04232</v>
       </c>
       <c r="F10">
-        <v>78.48999786376953</v>
+        <v>79.33499908447266</v>
       </c>
       <c r="G10">
-        <v>-0.5954927066039959</v>
+        <v>0.4751238400268634</v>
       </c>
       <c r="H10">
-        <v>-0.595240800697141</v>
+        <v>0.4749228526756111</v>
       </c>
       <c r="I10">
-        <v>0.8799972534179688</v>
+        <v>0.08499908447265625</v>
       </c>
       <c r="J10">
-        <v>1.13</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -786,19 +792,19 @@
         <v>100.00515</v>
       </c>
       <c r="F11">
-        <v>126.2057037353516</v>
+        <v>125.5192031860352</v>
       </c>
       <c r="G11">
-        <v>1.590441506958005</v>
+        <v>1.037808564758298</v>
       </c>
       <c r="H11">
-        <v>1.590359603438428</v>
+        <v>1.037755120369598</v>
       </c>
       <c r="I11">
-        <v>1.195701599121094</v>
+        <v>0.2392044067382812</v>
       </c>
       <c r="J11">
-        <v>0.96</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -818,19 +824,19 @@
         <v>100.01101</v>
       </c>
       <c r="F12">
-        <v>28.51499938964844</v>
+        <v>28.77239990234375</v>
       </c>
       <c r="G12">
-        <v>-1.43465710998535</v>
+        <v>-0.5448235375976552</v>
       </c>
       <c r="H12">
-        <v>-1.434499171626554</v>
+        <v>-0.5447635591297951</v>
       </c>
       <c r="I12">
-        <v>-0.005001068115234375</v>
+        <v>0.2323989868164062</v>
       </c>
       <c r="J12">
-        <v>-0.02</v>
+        <v>0.8100000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -850,19 +856,83 @@
         <v>99.93547999999998</v>
       </c>
       <c r="F13">
-        <v>47.43000030517578</v>
+        <v>48.03979873657227</v>
       </c>
       <c r="G13">
-        <v>-3.08341937683105</v>
+        <v>-1.838210979919429</v>
       </c>
       <c r="H13">
-        <v>-3.085410083416871</v>
+        <v>-1.839397759353764</v>
       </c>
       <c r="I13">
-        <v>0.1199989318847656</v>
+        <v>0.3097991943359375</v>
       </c>
       <c r="J13">
-        <v>0.25</v>
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>236.32</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>945.28</v>
+      </c>
+      <c r="F14">
+        <v>229.6900024414062</v>
+      </c>
+      <c r="G14">
+        <v>-26.51999023437497</v>
+      </c>
+      <c r="H14">
+        <v>-2.805516908680494</v>
+      </c>
+      <c r="I14">
+        <v>0.760009765625</v>
+      </c>
+      <c r="J14">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15">
+        <v>556.53</v>
+      </c>
+      <c r="D15">
+        <v>0.44921</v>
+      </c>
+      <c r="E15">
+        <v>249.9988413</v>
+      </c>
+      <c r="F15">
+        <v>558.5549926757812</v>
+      </c>
+      <c r="G15">
+        <v>0.9096469598877076</v>
+      </c>
+      <c r="H15">
+        <v>0.3638604703755911</v>
+      </c>
+      <c r="I15">
+        <v>3.7449951171875</v>
+      </c>
+      <c r="J15">
+        <v>0.68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>